<commit_message>
Object dection input variables integrated in database
</commit_message>
<xml_diff>
--- a/Database/CoastSnapDB.xlsx
+++ b/Database/CoastSnapDB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Coastal Citizen Science\CoastSnap\Database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\CoastSnap\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DEDE068-A13C-4874-8CD7-316050839D68}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EFA28E7-E4D2-4A2F-9EDA-FD3839222DAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-18855" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3384" yWindow="1956" windowWidth="17280" windowHeight="8976" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="database" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1288" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1311" uniqueCount="359">
   <si>
     <t>Site</t>
   </si>
@@ -1071,6 +1071,51 @@
   </si>
   <si>
     <t>[1 2 3]</t>
+  </si>
+  <si>
+    <t>Object Detection</t>
+  </si>
+  <si>
+    <t>Object Names</t>
+  </si>
+  <si>
+    <t>Models</t>
+  </si>
+  <si>
+    <t>Names of folder/objects as trained and stored (e.g. ['restaurant1', 'stairs1', 'stairs2'])</t>
+  </si>
+  <si>
+    <t>Filenames of detection models that are to be used. Should be in same order as Object names.</t>
+  </si>
+  <si>
+    <t>GCP's reference image</t>
+  </si>
+  <si>
+    <t>This should contain the pixel values of the GCP Rectification Combo for the Master Reference Image</t>
+  </si>
+  <si>
+    <t>UV-x</t>
+  </si>
+  <si>
+    <t>UV-y</t>
+  </si>
+  <si>
+    <t>Vertical pixel value</t>
+  </si>
+  <si>
+    <t>Horizontal pixel value</t>
+  </si>
+  <si>
+    <t>Reference Image</t>
+  </si>
+  <si>
+    <t>target_image23.jpg</t>
+  </si>
+  <si>
+    <t>strandtent,zilvermeeuw</t>
+  </si>
+  <si>
+    <t>detection_model-ex-016--loss-0008.891.h5,detection_model-ex-005--loss-0016.168.h5</t>
   </si>
 </sst>
 </file>
@@ -1083,7 +1128,7 @@
     <numFmt numFmtId="166" formatCode="#,##0.000"/>
     <numFmt numFmtId="167" formatCode="dd\/mm\/yyyy\ hh:mm"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1207,6 +1252,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="10">
     <fill>
@@ -1306,7 +1357,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1425,6 +1476,15 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="166" fontId="15" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="15" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="15" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -20390,7 +20450,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C82C2A5-FA5F-4BBC-B066-D9DA22911E90}">
   <dimension ref="A1:Z993"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
       <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
@@ -20934,7 +20994,7 @@
       <c r="W16" s="48"/>
       <c r="X16" s="48"/>
     </row>
-    <row r="17" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="48" t="s">
         <v>36</v>
       </c>
@@ -20968,7 +21028,7 @@
       <c r="W17" s="48"/>
       <c r="X17" s="48"/>
     </row>
-    <row r="18" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="48" t="s">
         <v>37</v>
       </c>
@@ -20981,28 +21041,30 @@
       <c r="D18" s="49" t="s">
         <v>86</v>
       </c>
-      <c r="E18" s="48"/>
-      <c r="F18" s="48"/>
-      <c r="G18" s="48"/>
-      <c r="H18" s="48"/>
-      <c r="I18" s="48"/>
-      <c r="J18" s="48"/>
-      <c r="K18" s="48"/>
-      <c r="L18" s="48"/>
-      <c r="M18" s="48"/>
-      <c r="N18" s="48"/>
-      <c r="O18" s="48"/>
-      <c r="P18" s="48"/>
-      <c r="Q18" s="48"/>
-      <c r="R18" s="48"/>
-      <c r="S18" s="48"/>
-      <c r="T18" s="48"/>
-      <c r="U18" s="48"/>
-      <c r="V18" s="48"/>
-      <c r="W18" s="48"/>
-      <c r="X18" s="48"/>
-    </row>
-    <row r="19" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E18" s="83"/>
+      <c r="F18" s="83"/>
+      <c r="G18" s="83"/>
+      <c r="H18" s="83"/>
+      <c r="I18" s="83"/>
+      <c r="J18" s="83"/>
+      <c r="K18" s="83"/>
+      <c r="L18" s="83"/>
+      <c r="M18" s="83"/>
+      <c r="N18" s="83"/>
+      <c r="O18" s="83"/>
+      <c r="P18" s="83"/>
+      <c r="Q18" s="83"/>
+      <c r="R18" s="83"/>
+      <c r="S18" s="83"/>
+      <c r="T18" s="83"/>
+      <c r="U18" s="83"/>
+      <c r="V18" s="83"/>
+      <c r="W18" s="83"/>
+      <c r="X18" s="83"/>
+      <c r="Y18" s="84"/>
+      <c r="Z18" s="84"/>
+    </row>
+    <row r="19" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="48" t="s">
         <v>87</v>
       </c>
@@ -21015,28 +21077,30 @@
       <c r="D19" s="48" t="s">
         <v>89</v>
       </c>
-      <c r="E19" s="48"/>
-      <c r="F19" s="48"/>
-      <c r="G19" s="48"/>
-      <c r="H19" s="48"/>
-      <c r="I19" s="48"/>
-      <c r="J19" s="48"/>
-      <c r="K19" s="48"/>
-      <c r="L19" s="48"/>
-      <c r="M19" s="48"/>
-      <c r="N19" s="48"/>
-      <c r="O19" s="48"/>
-      <c r="P19" s="48"/>
-      <c r="Q19" s="48"/>
-      <c r="R19" s="48"/>
-      <c r="S19" s="48"/>
-      <c r="T19" s="48"/>
-      <c r="U19" s="48"/>
-      <c r="V19" s="48"/>
-      <c r="W19" s="48"/>
-      <c r="X19" s="48"/>
-    </row>
-    <row r="20" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E19" s="83"/>
+      <c r="F19" s="83"/>
+      <c r="G19" s="83"/>
+      <c r="H19" s="83"/>
+      <c r="I19" s="83"/>
+      <c r="J19" s="83"/>
+      <c r="K19" s="83"/>
+      <c r="L19" s="83"/>
+      <c r="M19" s="83"/>
+      <c r="N19" s="83"/>
+      <c r="O19" s="83"/>
+      <c r="P19" s="83"/>
+      <c r="Q19" s="83"/>
+      <c r="R19" s="83"/>
+      <c r="S19" s="83"/>
+      <c r="T19" s="83"/>
+      <c r="U19" s="83"/>
+      <c r="V19" s="83"/>
+      <c r="W19" s="83"/>
+      <c r="X19" s="83"/>
+      <c r="Y19" s="84"/>
+      <c r="Z19" s="84"/>
+    </row>
+    <row r="20" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="48" t="s">
         <v>90</v>
       </c>
@@ -21049,28 +21113,30 @@
       <c r="D20" s="48" t="s">
         <v>91</v>
       </c>
-      <c r="E20" s="48"/>
-      <c r="F20" s="48"/>
-      <c r="G20" s="48"/>
-      <c r="H20" s="48"/>
-      <c r="I20" s="48"/>
-      <c r="J20" s="48"/>
-      <c r="K20" s="48"/>
-      <c r="L20" s="48"/>
-      <c r="M20" s="48"/>
-      <c r="N20" s="48"/>
-      <c r="O20" s="48"/>
-      <c r="P20" s="48"/>
-      <c r="Q20" s="48"/>
-      <c r="R20" s="48"/>
-      <c r="S20" s="48"/>
-      <c r="T20" s="48"/>
-      <c r="U20" s="48"/>
-      <c r="V20" s="48"/>
-      <c r="W20" s="48"/>
-      <c r="X20" s="48"/>
-    </row>
-    <row r="21" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E20" s="83"/>
+      <c r="F20" s="83"/>
+      <c r="G20" s="83"/>
+      <c r="H20" s="83"/>
+      <c r="I20" s="83"/>
+      <c r="J20" s="83"/>
+      <c r="K20" s="83"/>
+      <c r="L20" s="83"/>
+      <c r="M20" s="83"/>
+      <c r="N20" s="83"/>
+      <c r="O20" s="83"/>
+      <c r="P20" s="83"/>
+      <c r="Q20" s="83"/>
+      <c r="R20" s="83"/>
+      <c r="S20" s="83"/>
+      <c r="T20" s="83"/>
+      <c r="U20" s="83"/>
+      <c r="V20" s="83"/>
+      <c r="W20" s="83"/>
+      <c r="X20" s="83"/>
+      <c r="Y20" s="84"/>
+      <c r="Z20" s="84"/>
+    </row>
+    <row r="21" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="49" t="s">
         <v>92</v>
       </c>
@@ -21083,28 +21149,30 @@
       <c r="D21" s="48" t="s">
         <v>94</v>
       </c>
-      <c r="E21" s="48"/>
-      <c r="F21" s="48"/>
-      <c r="G21" s="48"/>
-      <c r="H21" s="48"/>
-      <c r="I21" s="48"/>
-      <c r="J21" s="48"/>
-      <c r="K21" s="48"/>
-      <c r="L21" s="48"/>
-      <c r="M21" s="48"/>
-      <c r="N21" s="48"/>
-      <c r="O21" s="48"/>
-      <c r="P21" s="48"/>
-      <c r="Q21" s="48"/>
-      <c r="R21" s="48"/>
-      <c r="S21" s="48"/>
-      <c r="T21" s="48"/>
-      <c r="U21" s="48"/>
-      <c r="V21" s="48"/>
-      <c r="W21" s="48"/>
-      <c r="X21" s="48"/>
-    </row>
-    <row r="22" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E21" s="83"/>
+      <c r="F21" s="83"/>
+      <c r="G21" s="83"/>
+      <c r="H21" s="83"/>
+      <c r="I21" s="83"/>
+      <c r="J21" s="83"/>
+      <c r="K21" s="83"/>
+      <c r="L21" s="83"/>
+      <c r="M21" s="83"/>
+      <c r="N21" s="83"/>
+      <c r="O21" s="83"/>
+      <c r="P21" s="83"/>
+      <c r="Q21" s="83"/>
+      <c r="R21" s="83"/>
+      <c r="S21" s="83"/>
+      <c r="T21" s="83"/>
+      <c r="U21" s="83"/>
+      <c r="V21" s="83"/>
+      <c r="W21" s="83"/>
+      <c r="X21" s="83"/>
+      <c r="Y21" s="84"/>
+      <c r="Z21" s="84"/>
+    </row>
+    <row r="22" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="48" t="s">
         <v>38</v>
       </c>
@@ -21117,56 +21185,60 @@
       <c r="D22" s="49" t="s">
         <v>118</v>
       </c>
-      <c r="E22" s="48"/>
-      <c r="F22" s="48"/>
-      <c r="G22" s="48"/>
-      <c r="H22" s="48"/>
-      <c r="I22" s="48"/>
-      <c r="J22" s="48"/>
-      <c r="K22" s="48"/>
-      <c r="L22" s="48"/>
-      <c r="M22" s="48"/>
-      <c r="N22" s="48"/>
-      <c r="O22" s="48"/>
-      <c r="P22" s="48"/>
-      <c r="Q22" s="48"/>
-      <c r="R22" s="48"/>
-      <c r="S22" s="48"/>
-      <c r="T22" s="48"/>
-      <c r="U22" s="48"/>
-      <c r="V22" s="48"/>
-      <c r="W22" s="48"/>
-      <c r="X22" s="48"/>
-    </row>
-    <row r="23" spans="1:24" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="E22" s="83"/>
+      <c r="F22" s="83"/>
+      <c r="G22" s="83"/>
+      <c r="H22" s="83"/>
+      <c r="I22" s="83"/>
+      <c r="J22" s="83"/>
+      <c r="K22" s="83"/>
+      <c r="L22" s="83"/>
+      <c r="M22" s="83"/>
+      <c r="N22" s="83"/>
+      <c r="O22" s="83"/>
+      <c r="P22" s="83"/>
+      <c r="Q22" s="83"/>
+      <c r="R22" s="83"/>
+      <c r="S22" s="83"/>
+      <c r="T22" s="83"/>
+      <c r="U22" s="83"/>
+      <c r="V22" s="83"/>
+      <c r="W22" s="83"/>
+      <c r="X22" s="83"/>
+      <c r="Y22" s="84"/>
+      <c r="Z22" s="84"/>
+    </row>
+    <row r="23" spans="1:26" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A23" s="10" t="s">
         <v>39</v>
       </c>
       <c r="B23" s="11"/>
       <c r="C23" s="11"/>
       <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="11"/>
-      <c r="K23" s="11"/>
-      <c r="L23" s="11"/>
-      <c r="M23" s="11"/>
-      <c r="N23" s="11"/>
-      <c r="O23" s="11"/>
-      <c r="P23" s="11"/>
-      <c r="Q23" s="11"/>
-      <c r="R23" s="11"/>
-      <c r="S23" s="11"/>
-      <c r="T23" s="11"/>
-      <c r="U23" s="11"/>
-      <c r="V23" s="11"/>
-      <c r="W23" s="11"/>
-      <c r="X23" s="11"/>
-    </row>
-    <row r="24" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E23" s="85"/>
+      <c r="F23" s="85"/>
+      <c r="G23" s="85"/>
+      <c r="H23" s="85"/>
+      <c r="I23" s="85"/>
+      <c r="J23" s="85"/>
+      <c r="K23" s="85"/>
+      <c r="L23" s="85"/>
+      <c r="M23" s="85"/>
+      <c r="N23" s="85"/>
+      <c r="O23" s="85"/>
+      <c r="P23" s="85"/>
+      <c r="Q23" s="85"/>
+      <c r="R23" s="85"/>
+      <c r="S23" s="85"/>
+      <c r="T23" s="85"/>
+      <c r="U23" s="85"/>
+      <c r="V23" s="85"/>
+      <c r="W23" s="85"/>
+      <c r="X23" s="85"/>
+      <c r="Y23" s="84"/>
+      <c r="Z23" s="84"/>
+    </row>
+    <row r="24" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="50" t="s">
         <v>40</v>
       </c>
@@ -21177,28 +21249,30 @@
       <c r="D24" s="52" t="s">
         <v>103</v>
       </c>
-      <c r="E24" s="52"/>
-      <c r="F24" s="52"/>
-      <c r="G24" s="52"/>
-      <c r="H24" s="52"/>
-      <c r="I24" s="52"/>
-      <c r="J24" s="52"/>
-      <c r="K24" s="52"/>
-      <c r="L24" s="52"/>
-      <c r="M24" s="52"/>
-      <c r="N24" s="52"/>
-      <c r="O24" s="52"/>
-      <c r="P24" s="52"/>
-      <c r="Q24" s="52"/>
-      <c r="R24" s="52"/>
-      <c r="S24" s="52"/>
-      <c r="T24" s="52"/>
-      <c r="U24" s="52"/>
-      <c r="V24" s="52"/>
-      <c r="W24" s="52"/>
-      <c r="X24" s="52"/>
-    </row>
-    <row r="25" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E24" s="85"/>
+      <c r="F24" s="85"/>
+      <c r="G24" s="85"/>
+      <c r="H24" s="85"/>
+      <c r="I24" s="85"/>
+      <c r="J24" s="85"/>
+      <c r="K24" s="85"/>
+      <c r="L24" s="85"/>
+      <c r="M24" s="85"/>
+      <c r="N24" s="85"/>
+      <c r="O24" s="85"/>
+      <c r="P24" s="85"/>
+      <c r="Q24" s="85"/>
+      <c r="R24" s="85"/>
+      <c r="S24" s="85"/>
+      <c r="T24" s="85"/>
+      <c r="U24" s="85"/>
+      <c r="V24" s="85"/>
+      <c r="W24" s="85"/>
+      <c r="X24" s="85"/>
+      <c r="Y24" s="84"/>
+      <c r="Z24" s="84"/>
+    </row>
+    <row r="25" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="50" t="s">
         <v>42</v>
       </c>
@@ -21211,56 +21285,60 @@
       <c r="D25" s="52" t="s">
         <v>104</v>
       </c>
-      <c r="E25" s="52"/>
-      <c r="F25" s="52"/>
-      <c r="G25" s="52"/>
-      <c r="H25" s="52"/>
-      <c r="I25" s="52"/>
-      <c r="J25" s="52"/>
-      <c r="K25" s="52"/>
-      <c r="L25" s="52"/>
-      <c r="M25" s="52"/>
-      <c r="N25" s="52"/>
-      <c r="O25" s="52"/>
-      <c r="P25" s="52"/>
-      <c r="Q25" s="52"/>
-      <c r="R25" s="52"/>
-      <c r="S25" s="52"/>
-      <c r="T25" s="52"/>
-      <c r="U25" s="52"/>
-      <c r="V25" s="52"/>
-      <c r="W25" s="52"/>
-      <c r="X25" s="52"/>
-    </row>
-    <row r="26" spans="1:24" ht="28.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="E25" s="85"/>
+      <c r="F25" s="85"/>
+      <c r="G25" s="85"/>
+      <c r="H25" s="85"/>
+      <c r="I25" s="85"/>
+      <c r="J25" s="85"/>
+      <c r="K25" s="85"/>
+      <c r="L25" s="85"/>
+      <c r="M25" s="85"/>
+      <c r="N25" s="85"/>
+      <c r="O25" s="85"/>
+      <c r="P25" s="85"/>
+      <c r="Q25" s="85"/>
+      <c r="R25" s="85"/>
+      <c r="S25" s="85"/>
+      <c r="T25" s="85"/>
+      <c r="U25" s="85"/>
+      <c r="V25" s="85"/>
+      <c r="W25" s="85"/>
+      <c r="X25" s="85"/>
+      <c r="Y25" s="84"/>
+      <c r="Z25" s="84"/>
+    </row>
+    <row r="26" spans="1:26" ht="28.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A26" s="17" t="s">
         <v>45</v>
       </c>
       <c r="B26" s="18"/>
       <c r="C26" s="18"/>
       <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
-      <c r="H26" s="18"/>
-      <c r="I26" s="18"/>
-      <c r="J26" s="18"/>
-      <c r="K26" s="18"/>
-      <c r="L26" s="18"/>
-      <c r="M26" s="18"/>
-      <c r="N26" s="18"/>
-      <c r="O26" s="18"/>
-      <c r="P26" s="18"/>
-      <c r="Q26" s="18"/>
-      <c r="R26" s="18"/>
-      <c r="S26" s="18"/>
-      <c r="T26" s="18"/>
-      <c r="U26" s="18"/>
-      <c r="V26" s="18"/>
-      <c r="W26" s="18"/>
-      <c r="X26" s="18"/>
-    </row>
-    <row r="27" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E26" s="86"/>
+      <c r="F26" s="86"/>
+      <c r="G26" s="86"/>
+      <c r="H26" s="86"/>
+      <c r="I26" s="86"/>
+      <c r="J26" s="86"/>
+      <c r="K26" s="86"/>
+      <c r="L26" s="86"/>
+      <c r="M26" s="86"/>
+      <c r="N26" s="86"/>
+      <c r="O26" s="86"/>
+      <c r="P26" s="86"/>
+      <c r="Q26" s="86"/>
+      <c r="R26" s="86"/>
+      <c r="S26" s="86"/>
+      <c r="T26" s="86"/>
+      <c r="U26" s="86"/>
+      <c r="V26" s="86"/>
+      <c r="W26" s="86"/>
+      <c r="X26" s="86"/>
+      <c r="Y26" s="84"/>
+      <c r="Z26" s="84"/>
+    </row>
+    <row r="27" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="53" t="s">
         <v>46</v>
       </c>
@@ -21271,28 +21349,30 @@
       <c r="D27" s="55" t="s">
         <v>98</v>
       </c>
-      <c r="E27" s="55"/>
-      <c r="F27" s="55"/>
-      <c r="G27" s="55"/>
-      <c r="H27" s="55"/>
-      <c r="I27" s="55"/>
-      <c r="J27" s="55"/>
-      <c r="K27" s="55"/>
-      <c r="L27" s="55"/>
-      <c r="M27" s="55"/>
-      <c r="N27" s="55"/>
-      <c r="O27" s="55"/>
-      <c r="P27" s="55"/>
-      <c r="Q27" s="55"/>
-      <c r="R27" s="55"/>
-      <c r="S27" s="55"/>
-      <c r="T27" s="55"/>
-      <c r="U27" s="55"/>
-      <c r="V27" s="55"/>
-      <c r="W27" s="55"/>
-      <c r="X27" s="55"/>
-    </row>
-    <row r="28" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E27" s="86"/>
+      <c r="F27" s="86"/>
+      <c r="G27" s="86"/>
+      <c r="H27" s="86"/>
+      <c r="I27" s="86"/>
+      <c r="J27" s="86"/>
+      <c r="K27" s="86"/>
+      <c r="L27" s="86"/>
+      <c r="M27" s="86"/>
+      <c r="N27" s="86"/>
+      <c r="O27" s="86"/>
+      <c r="P27" s="86"/>
+      <c r="Q27" s="86"/>
+      <c r="R27" s="86"/>
+      <c r="S27" s="86"/>
+      <c r="T27" s="86"/>
+      <c r="U27" s="86"/>
+      <c r="V27" s="86"/>
+      <c r="W27" s="86"/>
+      <c r="X27" s="86"/>
+      <c r="Y27" s="84"/>
+      <c r="Z27" s="84"/>
+    </row>
+    <row r="28" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="53" t="s">
         <v>73</v>
       </c>
@@ -21303,28 +21383,30 @@
       <c r="D28" s="53" t="s">
         <v>96</v>
       </c>
-      <c r="E28" s="55"/>
-      <c r="F28" s="55"/>
-      <c r="G28" s="55"/>
-      <c r="H28" s="55"/>
-      <c r="I28" s="55"/>
-      <c r="J28" s="55"/>
-      <c r="K28" s="55"/>
-      <c r="L28" s="55"/>
-      <c r="M28" s="55"/>
-      <c r="N28" s="55"/>
-      <c r="O28" s="55"/>
-      <c r="P28" s="55"/>
-      <c r="Q28" s="55"/>
-      <c r="R28" s="55"/>
-      <c r="S28" s="55"/>
-      <c r="T28" s="55"/>
-      <c r="U28" s="55"/>
-      <c r="V28" s="55"/>
-      <c r="W28" s="55"/>
-      <c r="X28" s="55"/>
-    </row>
-    <row r="29" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E28" s="86"/>
+      <c r="F28" s="86"/>
+      <c r="G28" s="86"/>
+      <c r="H28" s="86"/>
+      <c r="I28" s="86"/>
+      <c r="J28" s="86"/>
+      <c r="K28" s="86"/>
+      <c r="L28" s="86"/>
+      <c r="M28" s="86"/>
+      <c r="N28" s="86"/>
+      <c r="O28" s="86"/>
+      <c r="P28" s="86"/>
+      <c r="Q28" s="86"/>
+      <c r="R28" s="86"/>
+      <c r="S28" s="86"/>
+      <c r="T28" s="86"/>
+      <c r="U28" s="86"/>
+      <c r="V28" s="86"/>
+      <c r="W28" s="86"/>
+      <c r="X28" s="86"/>
+      <c r="Y28" s="84"/>
+      <c r="Z28" s="84"/>
+    </row>
+    <row r="29" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="53" t="s">
         <v>74</v>
       </c>
@@ -21335,28 +21417,30 @@
       <c r="D29" s="53" t="s">
         <v>97</v>
       </c>
-      <c r="E29" s="55"/>
-      <c r="F29" s="55"/>
-      <c r="G29" s="55"/>
-      <c r="H29" s="55"/>
-      <c r="I29" s="55"/>
-      <c r="J29" s="55"/>
-      <c r="K29" s="55"/>
-      <c r="L29" s="55"/>
-      <c r="M29" s="55"/>
-      <c r="N29" s="55"/>
-      <c r="O29" s="55"/>
-      <c r="P29" s="55"/>
-      <c r="Q29" s="55"/>
-      <c r="R29" s="55"/>
-      <c r="S29" s="55"/>
-      <c r="T29" s="55"/>
-      <c r="U29" s="55"/>
-      <c r="V29" s="55"/>
-      <c r="W29" s="55"/>
-      <c r="X29" s="55"/>
-    </row>
-    <row r="30" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="E29" s="86"/>
+      <c r="F29" s="86"/>
+      <c r="G29" s="86"/>
+      <c r="H29" s="86"/>
+      <c r="I29" s="86"/>
+      <c r="J29" s="86"/>
+      <c r="K29" s="86"/>
+      <c r="L29" s="86"/>
+      <c r="M29" s="86"/>
+      <c r="N29" s="86"/>
+      <c r="O29" s="86"/>
+      <c r="P29" s="86"/>
+      <c r="Q29" s="86"/>
+      <c r="R29" s="86"/>
+      <c r="S29" s="86"/>
+      <c r="T29" s="86"/>
+      <c r="U29" s="86"/>
+      <c r="V29" s="86"/>
+      <c r="W29" s="86"/>
+      <c r="X29" s="86"/>
+      <c r="Y29" s="84"/>
+      <c r="Z29" s="84"/>
+    </row>
+    <row r="30" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A30" s="22" t="s">
         <v>48</v>
       </c>
@@ -21365,28 +21449,30 @@
       <c r="D30" s="58" t="s">
         <v>99</v>
       </c>
-      <c r="E30" s="56"/>
-      <c r="F30" s="56"/>
-      <c r="G30" s="56"/>
-      <c r="H30" s="56"/>
-      <c r="I30" s="56"/>
-      <c r="J30" s="56"/>
-      <c r="K30" s="56"/>
-      <c r="L30" s="56"/>
-      <c r="M30" s="56"/>
-      <c r="N30" s="56"/>
-      <c r="O30" s="56"/>
-      <c r="P30" s="56"/>
-      <c r="Q30" s="56"/>
-      <c r="R30" s="56"/>
-      <c r="S30" s="56"/>
-      <c r="T30" s="56"/>
-      <c r="U30" s="56"/>
-      <c r="V30" s="56"/>
-      <c r="W30" s="56"/>
-      <c r="X30" s="56"/>
-    </row>
-    <row r="31" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E30" s="87"/>
+      <c r="F30" s="87"/>
+      <c r="G30" s="87"/>
+      <c r="H30" s="87"/>
+      <c r="I30" s="87"/>
+      <c r="J30" s="87"/>
+      <c r="K30" s="87"/>
+      <c r="L30" s="87"/>
+      <c r="M30" s="87"/>
+      <c r="N30" s="87"/>
+      <c r="O30" s="87"/>
+      <c r="P30" s="87"/>
+      <c r="Q30" s="87"/>
+      <c r="R30" s="87"/>
+      <c r="S30" s="87"/>
+      <c r="T30" s="87"/>
+      <c r="U30" s="87"/>
+      <c r="V30" s="87"/>
+      <c r="W30" s="87"/>
+      <c r="X30" s="87"/>
+      <c r="Y30" s="84"/>
+      <c r="Z30" s="84"/>
+    </row>
+    <row r="31" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="56" t="s">
         <v>49</v>
       </c>
@@ -21397,28 +21483,30 @@
       <c r="D31" s="56" t="s">
         <v>105</v>
       </c>
-      <c r="E31" s="56"/>
-      <c r="F31" s="56"/>
-      <c r="G31" s="56"/>
-      <c r="H31" s="56"/>
-      <c r="I31" s="56"/>
-      <c r="J31" s="56"/>
-      <c r="K31" s="56"/>
-      <c r="L31" s="56"/>
-      <c r="M31" s="56"/>
-      <c r="N31" s="56"/>
-      <c r="O31" s="56"/>
-      <c r="P31" s="56"/>
-      <c r="Q31" s="56"/>
-      <c r="R31" s="56"/>
-      <c r="S31" s="56"/>
-      <c r="T31" s="56"/>
-      <c r="U31" s="56"/>
-      <c r="V31" s="56"/>
-      <c r="W31" s="56"/>
-      <c r="X31" s="56"/>
-    </row>
-    <row r="32" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E31" s="87"/>
+      <c r="F31" s="87"/>
+      <c r="G31" s="87"/>
+      <c r="H31" s="87"/>
+      <c r="I31" s="87"/>
+      <c r="J31" s="87"/>
+      <c r="K31" s="87"/>
+      <c r="L31" s="87"/>
+      <c r="M31" s="87"/>
+      <c r="N31" s="87"/>
+      <c r="O31" s="87"/>
+      <c r="P31" s="87"/>
+      <c r="Q31" s="87"/>
+      <c r="R31" s="87"/>
+      <c r="S31" s="87"/>
+      <c r="T31" s="87"/>
+      <c r="U31" s="87"/>
+      <c r="V31" s="87"/>
+      <c r="W31" s="87"/>
+      <c r="X31" s="87"/>
+      <c r="Y31" s="84"/>
+      <c r="Z31" s="84"/>
+    </row>
+    <row r="32" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="56" t="s">
         <v>9</v>
       </c>
@@ -21431,28 +21519,30 @@
       <c r="D32" s="56" t="s">
         <v>106</v>
       </c>
-      <c r="E32" s="56"/>
-      <c r="F32" s="56"/>
-      <c r="G32" s="56"/>
-      <c r="H32" s="56"/>
-      <c r="I32" s="56"/>
-      <c r="J32" s="56"/>
-      <c r="K32" s="56"/>
-      <c r="L32" s="56"/>
-      <c r="M32" s="56"/>
-      <c r="N32" s="56"/>
-      <c r="O32" s="56"/>
-      <c r="P32" s="56"/>
-      <c r="Q32" s="56"/>
-      <c r="R32" s="56"/>
-      <c r="S32" s="56"/>
-      <c r="T32" s="56"/>
-      <c r="U32" s="56"/>
-      <c r="V32" s="56"/>
-      <c r="W32" s="56"/>
-      <c r="X32" s="56"/>
-    </row>
-    <row r="33" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E32" s="87"/>
+      <c r="F32" s="87"/>
+      <c r="G32" s="87"/>
+      <c r="H32" s="87"/>
+      <c r="I32" s="87"/>
+      <c r="J32" s="87"/>
+      <c r="K32" s="87"/>
+      <c r="L32" s="87"/>
+      <c r="M32" s="87"/>
+      <c r="N32" s="87"/>
+      <c r="O32" s="87"/>
+      <c r="P32" s="87"/>
+      <c r="Q32" s="87"/>
+      <c r="R32" s="87"/>
+      <c r="S32" s="87"/>
+      <c r="T32" s="87"/>
+      <c r="U32" s="87"/>
+      <c r="V32" s="87"/>
+      <c r="W32" s="87"/>
+      <c r="X32" s="87"/>
+      <c r="Y32" s="84"/>
+      <c r="Z32" s="84"/>
+    </row>
+    <row r="33" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="56" t="s">
         <v>12</v>
       </c>
@@ -21465,28 +21555,30 @@
       <c r="D33" s="56" t="s">
         <v>106</v>
       </c>
-      <c r="E33" s="56"/>
-      <c r="F33" s="56"/>
-      <c r="G33" s="56"/>
-      <c r="H33" s="56"/>
-      <c r="I33" s="56"/>
-      <c r="J33" s="56"/>
-      <c r="K33" s="56"/>
-      <c r="L33" s="56"/>
-      <c r="M33" s="56"/>
-      <c r="N33" s="56"/>
-      <c r="O33" s="56"/>
-      <c r="P33" s="56"/>
-      <c r="Q33" s="56"/>
-      <c r="R33" s="56"/>
-      <c r="S33" s="56"/>
-      <c r="T33" s="56"/>
-      <c r="U33" s="56"/>
-      <c r="V33" s="56"/>
-      <c r="W33" s="56"/>
-      <c r="X33" s="56"/>
-    </row>
-    <row r="34" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E33" s="87"/>
+      <c r="F33" s="87"/>
+      <c r="G33" s="87"/>
+      <c r="H33" s="87"/>
+      <c r="I33" s="87"/>
+      <c r="J33" s="87"/>
+      <c r="K33" s="87"/>
+      <c r="L33" s="87"/>
+      <c r="M33" s="87"/>
+      <c r="N33" s="87"/>
+      <c r="O33" s="87"/>
+      <c r="P33" s="87"/>
+      <c r="Q33" s="87"/>
+      <c r="R33" s="87"/>
+      <c r="S33" s="87"/>
+      <c r="T33" s="87"/>
+      <c r="U33" s="87"/>
+      <c r="V33" s="87"/>
+      <c r="W33" s="87"/>
+      <c r="X33" s="87"/>
+      <c r="Y33" s="84"/>
+      <c r="Z33" s="84"/>
+    </row>
+    <row r="34" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="56" t="s">
         <v>15</v>
       </c>
@@ -21499,28 +21591,30 @@
       <c r="D34" s="56" t="s">
         <v>106</v>
       </c>
-      <c r="E34" s="56"/>
-      <c r="F34" s="56"/>
-      <c r="G34" s="56"/>
-      <c r="H34" s="56"/>
-      <c r="I34" s="56"/>
-      <c r="J34" s="56"/>
-      <c r="K34" s="56"/>
-      <c r="L34" s="56"/>
-      <c r="M34" s="56"/>
-      <c r="N34" s="56"/>
-      <c r="O34" s="56"/>
-      <c r="P34" s="56"/>
-      <c r="Q34" s="56"/>
-      <c r="R34" s="56"/>
-      <c r="S34" s="56"/>
-      <c r="T34" s="56"/>
-      <c r="U34" s="56"/>
-      <c r="V34" s="56"/>
-      <c r="W34" s="56"/>
-      <c r="X34" s="56"/>
-    </row>
-    <row r="35" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E34" s="87"/>
+      <c r="F34" s="87"/>
+      <c r="G34" s="87"/>
+      <c r="H34" s="87"/>
+      <c r="I34" s="87"/>
+      <c r="J34" s="87"/>
+      <c r="K34" s="87"/>
+      <c r="L34" s="87"/>
+      <c r="M34" s="87"/>
+      <c r="N34" s="87"/>
+      <c r="O34" s="87"/>
+      <c r="P34" s="87"/>
+      <c r="Q34" s="87"/>
+      <c r="R34" s="87"/>
+      <c r="S34" s="87"/>
+      <c r="T34" s="87"/>
+      <c r="U34" s="87"/>
+      <c r="V34" s="87"/>
+      <c r="W34" s="87"/>
+      <c r="X34" s="87"/>
+      <c r="Y34" s="84"/>
+      <c r="Z34" s="84"/>
+    </row>
+    <row r="35" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="56" t="s">
         <v>49</v>
       </c>
@@ -21531,28 +21625,30 @@
       <c r="D35" s="56" t="s">
         <v>105</v>
       </c>
-      <c r="E35" s="56"/>
-      <c r="F35" s="56"/>
-      <c r="G35" s="56"/>
-      <c r="H35" s="56"/>
-      <c r="I35" s="56"/>
-      <c r="J35" s="56"/>
-      <c r="K35" s="56"/>
-      <c r="L35" s="56"/>
-      <c r="M35" s="56"/>
-      <c r="N35" s="56"/>
-      <c r="O35" s="56"/>
-      <c r="P35" s="56"/>
-      <c r="Q35" s="56"/>
-      <c r="R35" s="56"/>
-      <c r="S35" s="56"/>
-      <c r="T35" s="56"/>
-      <c r="U35" s="56"/>
-      <c r="V35" s="56"/>
-      <c r="W35" s="56"/>
-      <c r="X35" s="56"/>
-    </row>
-    <row r="36" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E35" s="87"/>
+      <c r="F35" s="87"/>
+      <c r="G35" s="87"/>
+      <c r="H35" s="87"/>
+      <c r="I35" s="87"/>
+      <c r="J35" s="87"/>
+      <c r="K35" s="87"/>
+      <c r="L35" s="87"/>
+      <c r="M35" s="87"/>
+      <c r="N35" s="87"/>
+      <c r="O35" s="87"/>
+      <c r="P35" s="87"/>
+      <c r="Q35" s="87"/>
+      <c r="R35" s="87"/>
+      <c r="S35" s="87"/>
+      <c r="T35" s="87"/>
+      <c r="U35" s="87"/>
+      <c r="V35" s="87"/>
+      <c r="W35" s="87"/>
+      <c r="X35" s="87"/>
+      <c r="Y35" s="84"/>
+      <c r="Z35" s="84"/>
+    </row>
+    <row r="36" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="56" t="s">
         <v>9</v>
       </c>
@@ -21565,28 +21661,30 @@
       <c r="D36" s="56" t="s">
         <v>106</v>
       </c>
-      <c r="E36" s="56"/>
-      <c r="F36" s="56"/>
-      <c r="G36" s="56"/>
-      <c r="H36" s="56"/>
-      <c r="I36" s="56"/>
-      <c r="J36" s="56"/>
-      <c r="K36" s="56"/>
-      <c r="L36" s="56"/>
-      <c r="M36" s="56"/>
-      <c r="N36" s="56"/>
-      <c r="O36" s="56"/>
-      <c r="P36" s="56"/>
-      <c r="Q36" s="56"/>
-      <c r="R36" s="56"/>
-      <c r="S36" s="56"/>
-      <c r="T36" s="56"/>
-      <c r="U36" s="56"/>
-      <c r="V36" s="56"/>
-      <c r="W36" s="56"/>
-      <c r="X36" s="56"/>
-    </row>
-    <row r="37" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E36" s="87"/>
+      <c r="F36" s="87"/>
+      <c r="G36" s="87"/>
+      <c r="H36" s="87"/>
+      <c r="I36" s="87"/>
+      <c r="J36" s="87"/>
+      <c r="K36" s="87"/>
+      <c r="L36" s="87"/>
+      <c r="M36" s="87"/>
+      <c r="N36" s="87"/>
+      <c r="O36" s="87"/>
+      <c r="P36" s="87"/>
+      <c r="Q36" s="87"/>
+      <c r="R36" s="87"/>
+      <c r="S36" s="87"/>
+      <c r="T36" s="87"/>
+      <c r="U36" s="87"/>
+      <c r="V36" s="87"/>
+      <c r="W36" s="87"/>
+      <c r="X36" s="87"/>
+      <c r="Y36" s="84"/>
+      <c r="Z36" s="84"/>
+    </row>
+    <row r="37" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="56" t="s">
         <v>12</v>
       </c>
@@ -21599,28 +21697,30 @@
       <c r="D37" s="56" t="s">
         <v>106</v>
       </c>
-      <c r="E37" s="56"/>
-      <c r="F37" s="56"/>
-      <c r="G37" s="56"/>
-      <c r="H37" s="56"/>
-      <c r="I37" s="56"/>
-      <c r="J37" s="56"/>
-      <c r="K37" s="56"/>
-      <c r="L37" s="56"/>
-      <c r="M37" s="56"/>
-      <c r="N37" s="56"/>
-      <c r="O37" s="56"/>
-      <c r="P37" s="56"/>
-      <c r="Q37" s="56"/>
-      <c r="R37" s="56"/>
-      <c r="S37" s="56"/>
-      <c r="T37" s="56"/>
-      <c r="U37" s="56"/>
-      <c r="V37" s="56"/>
-      <c r="W37" s="56"/>
-      <c r="X37" s="56"/>
-    </row>
-    <row r="38" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E37" s="87"/>
+      <c r="F37" s="87"/>
+      <c r="G37" s="87"/>
+      <c r="H37" s="87"/>
+      <c r="I37" s="87"/>
+      <c r="J37" s="87"/>
+      <c r="K37" s="87"/>
+      <c r="L37" s="87"/>
+      <c r="M37" s="87"/>
+      <c r="N37" s="87"/>
+      <c r="O37" s="87"/>
+      <c r="P37" s="87"/>
+      <c r="Q37" s="87"/>
+      <c r="R37" s="87"/>
+      <c r="S37" s="87"/>
+      <c r="T37" s="87"/>
+      <c r="U37" s="87"/>
+      <c r="V37" s="87"/>
+      <c r="W37" s="87"/>
+      <c r="X37" s="87"/>
+      <c r="Y37" s="84"/>
+      <c r="Z37" s="84"/>
+    </row>
+    <row r="38" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="56" t="s">
         <v>15</v>
       </c>
@@ -21633,28 +21733,30 @@
       <c r="D38" s="56" t="s">
         <v>106</v>
       </c>
-      <c r="E38" s="56"/>
-      <c r="F38" s="56"/>
-      <c r="G38" s="56"/>
-      <c r="H38" s="56"/>
-      <c r="I38" s="56"/>
-      <c r="J38" s="56"/>
-      <c r="K38" s="56"/>
-      <c r="L38" s="56"/>
-      <c r="M38" s="56"/>
-      <c r="N38" s="56"/>
-      <c r="O38" s="56"/>
-      <c r="P38" s="56"/>
-      <c r="Q38" s="56"/>
-      <c r="R38" s="56"/>
-      <c r="S38" s="56"/>
-      <c r="T38" s="56"/>
-      <c r="U38" s="56"/>
-      <c r="V38" s="56"/>
-      <c r="W38" s="56"/>
-      <c r="X38" s="56"/>
-    </row>
-    <row r="39" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E38" s="87"/>
+      <c r="F38" s="87"/>
+      <c r="G38" s="87"/>
+      <c r="H38" s="87"/>
+      <c r="I38" s="87"/>
+      <c r="J38" s="87"/>
+      <c r="K38" s="87"/>
+      <c r="L38" s="87"/>
+      <c r="M38" s="87"/>
+      <c r="N38" s="87"/>
+      <c r="O38" s="87"/>
+      <c r="P38" s="87"/>
+      <c r="Q38" s="87"/>
+      <c r="R38" s="87"/>
+      <c r="S38" s="87"/>
+      <c r="T38" s="87"/>
+      <c r="U38" s="87"/>
+      <c r="V38" s="87"/>
+      <c r="W38" s="87"/>
+      <c r="X38" s="87"/>
+      <c r="Y38" s="84"/>
+      <c r="Z38" s="84"/>
+    </row>
+    <row r="39" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="56" t="s">
         <v>49</v>
       </c>
@@ -21665,28 +21767,30 @@
       <c r="D39" s="56" t="s">
         <v>105</v>
       </c>
-      <c r="E39" s="56"/>
-      <c r="F39" s="56"/>
-      <c r="G39" s="56"/>
-      <c r="H39" s="56"/>
-      <c r="I39" s="56"/>
-      <c r="J39" s="56"/>
-      <c r="K39" s="56"/>
-      <c r="L39" s="56"/>
-      <c r="M39" s="56"/>
-      <c r="N39" s="56"/>
-      <c r="O39" s="56"/>
-      <c r="P39" s="56"/>
-      <c r="Q39" s="56"/>
-      <c r="R39" s="56"/>
-      <c r="S39" s="56"/>
-      <c r="T39" s="56"/>
-      <c r="U39" s="56"/>
-      <c r="V39" s="56"/>
-      <c r="W39" s="56"/>
-      <c r="X39" s="56"/>
-    </row>
-    <row r="40" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E39" s="87"/>
+      <c r="F39" s="87"/>
+      <c r="G39" s="87"/>
+      <c r="H39" s="87"/>
+      <c r="I39" s="87"/>
+      <c r="J39" s="87"/>
+      <c r="K39" s="87"/>
+      <c r="L39" s="87"/>
+      <c r="M39" s="87"/>
+      <c r="N39" s="87"/>
+      <c r="O39" s="87"/>
+      <c r="P39" s="87"/>
+      <c r="Q39" s="87"/>
+      <c r="R39" s="87"/>
+      <c r="S39" s="87"/>
+      <c r="T39" s="87"/>
+      <c r="U39" s="87"/>
+      <c r="V39" s="87"/>
+      <c r="W39" s="87"/>
+      <c r="X39" s="87"/>
+      <c r="Y39" s="84"/>
+      <c r="Z39" s="84"/>
+    </row>
+    <row r="40" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="56" t="s">
         <v>9</v>
       </c>
@@ -21699,28 +21803,30 @@
       <c r="D40" s="56" t="s">
         <v>106</v>
       </c>
-      <c r="E40" s="56"/>
-      <c r="F40" s="56"/>
-      <c r="G40" s="56"/>
-      <c r="H40" s="56"/>
-      <c r="I40" s="56"/>
-      <c r="J40" s="56"/>
-      <c r="K40" s="56"/>
-      <c r="L40" s="56"/>
-      <c r="M40" s="56"/>
-      <c r="N40" s="56"/>
-      <c r="O40" s="56"/>
-      <c r="P40" s="56"/>
-      <c r="Q40" s="56"/>
-      <c r="R40" s="56"/>
-      <c r="S40" s="56"/>
-      <c r="T40" s="56"/>
-      <c r="U40" s="56"/>
-      <c r="V40" s="56"/>
-      <c r="W40" s="56"/>
-      <c r="X40" s="56"/>
-    </row>
-    <row r="41" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E40" s="87"/>
+      <c r="F40" s="87"/>
+      <c r="G40" s="87"/>
+      <c r="H40" s="87"/>
+      <c r="I40" s="87"/>
+      <c r="J40" s="87"/>
+      <c r="K40" s="87"/>
+      <c r="L40" s="87"/>
+      <c r="M40" s="87"/>
+      <c r="N40" s="87"/>
+      <c r="O40" s="87"/>
+      <c r="P40" s="87"/>
+      <c r="Q40" s="87"/>
+      <c r="R40" s="87"/>
+      <c r="S40" s="87"/>
+      <c r="T40" s="87"/>
+      <c r="U40" s="87"/>
+      <c r="V40" s="87"/>
+      <c r="W40" s="87"/>
+      <c r="X40" s="87"/>
+      <c r="Y40" s="84"/>
+      <c r="Z40" s="84"/>
+    </row>
+    <row r="41" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="56" t="s">
         <v>12</v>
       </c>
@@ -21733,28 +21839,30 @@
       <c r="D41" s="56" t="s">
         <v>106</v>
       </c>
-      <c r="E41" s="56"/>
-      <c r="F41" s="56"/>
-      <c r="G41" s="56"/>
-      <c r="H41" s="56"/>
-      <c r="I41" s="56"/>
-      <c r="J41" s="56"/>
-      <c r="K41" s="56"/>
-      <c r="L41" s="56"/>
-      <c r="M41" s="56"/>
-      <c r="N41" s="56"/>
-      <c r="O41" s="56"/>
-      <c r="P41" s="56"/>
-      <c r="Q41" s="56"/>
-      <c r="R41" s="56"/>
-      <c r="S41" s="56"/>
-      <c r="T41" s="56"/>
-      <c r="U41" s="56"/>
-      <c r="V41" s="56"/>
-      <c r="W41" s="56"/>
-      <c r="X41" s="56"/>
-    </row>
-    <row r="42" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E41" s="87"/>
+      <c r="F41" s="87"/>
+      <c r="G41" s="87"/>
+      <c r="H41" s="87"/>
+      <c r="I41" s="87"/>
+      <c r="J41" s="87"/>
+      <c r="K41" s="87"/>
+      <c r="L41" s="87"/>
+      <c r="M41" s="87"/>
+      <c r="N41" s="87"/>
+      <c r="O41" s="87"/>
+      <c r="P41" s="87"/>
+      <c r="Q41" s="87"/>
+      <c r="R41" s="87"/>
+      <c r="S41" s="87"/>
+      <c r="T41" s="87"/>
+      <c r="U41" s="87"/>
+      <c r="V41" s="87"/>
+      <c r="W41" s="87"/>
+      <c r="X41" s="87"/>
+      <c r="Y41" s="84"/>
+      <c r="Z41" s="84"/>
+    </row>
+    <row r="42" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="56" t="s">
         <v>15</v>
       </c>
@@ -21767,28 +21875,30 @@
       <c r="D42" s="56" t="s">
         <v>106</v>
       </c>
-      <c r="E42" s="56"/>
-      <c r="F42" s="56"/>
-      <c r="G42" s="56"/>
-      <c r="H42" s="56"/>
-      <c r="I42" s="56"/>
-      <c r="J42" s="56"/>
-      <c r="K42" s="56"/>
-      <c r="L42" s="56"/>
-      <c r="M42" s="56"/>
-      <c r="N42" s="56"/>
-      <c r="O42" s="56"/>
-      <c r="P42" s="56"/>
-      <c r="Q42" s="56"/>
-      <c r="R42" s="56"/>
-      <c r="S42" s="56"/>
-      <c r="T42" s="56"/>
-      <c r="U42" s="56"/>
-      <c r="V42" s="56"/>
-      <c r="W42" s="56"/>
-      <c r="X42" s="56"/>
-    </row>
-    <row r="43" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E42" s="87"/>
+      <c r="F42" s="87"/>
+      <c r="G42" s="87"/>
+      <c r="H42" s="87"/>
+      <c r="I42" s="87"/>
+      <c r="J42" s="87"/>
+      <c r="K42" s="87"/>
+      <c r="L42" s="87"/>
+      <c r="M42" s="87"/>
+      <c r="N42" s="87"/>
+      <c r="O42" s="87"/>
+      <c r="P42" s="87"/>
+      <c r="Q42" s="87"/>
+      <c r="R42" s="87"/>
+      <c r="S42" s="87"/>
+      <c r="T42" s="87"/>
+      <c r="U42" s="87"/>
+      <c r="V42" s="87"/>
+      <c r="W42" s="87"/>
+      <c r="X42" s="87"/>
+      <c r="Y42" s="84"/>
+      <c r="Z42" s="84"/>
+    </row>
+    <row r="43" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="56" t="s">
         <v>49</v>
       </c>
@@ -21799,28 +21909,30 @@
       <c r="D43" s="56" t="s">
         <v>105</v>
       </c>
-      <c r="E43" s="56"/>
-      <c r="F43" s="56"/>
-      <c r="G43" s="56"/>
-      <c r="H43" s="56"/>
-      <c r="I43" s="56"/>
-      <c r="J43" s="56"/>
-      <c r="K43" s="56"/>
-      <c r="L43" s="56"/>
-      <c r="M43" s="56"/>
-      <c r="N43" s="56"/>
-      <c r="O43" s="56"/>
-      <c r="P43" s="56"/>
-      <c r="Q43" s="56"/>
-      <c r="R43" s="56"/>
-      <c r="S43" s="56"/>
-      <c r="T43" s="56"/>
-      <c r="U43" s="56"/>
-      <c r="V43" s="56"/>
-      <c r="W43" s="56"/>
-      <c r="X43" s="56"/>
-    </row>
-    <row r="44" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E43" s="87"/>
+      <c r="F43" s="87"/>
+      <c r="G43" s="87"/>
+      <c r="H43" s="87"/>
+      <c r="I43" s="87"/>
+      <c r="J43" s="87"/>
+      <c r="K43" s="87"/>
+      <c r="L43" s="87"/>
+      <c r="M43" s="87"/>
+      <c r="N43" s="87"/>
+      <c r="O43" s="87"/>
+      <c r="P43" s="87"/>
+      <c r="Q43" s="87"/>
+      <c r="R43" s="87"/>
+      <c r="S43" s="87"/>
+      <c r="T43" s="87"/>
+      <c r="U43" s="87"/>
+      <c r="V43" s="87"/>
+      <c r="W43" s="87"/>
+      <c r="X43" s="87"/>
+      <c r="Y43" s="84"/>
+      <c r="Z43" s="84"/>
+    </row>
+    <row r="44" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="56" t="s">
         <v>9</v>
       </c>
@@ -21833,28 +21945,30 @@
       <c r="D44" s="56" t="s">
         <v>106</v>
       </c>
-      <c r="E44" s="56"/>
-      <c r="F44" s="56"/>
-      <c r="G44" s="56"/>
-      <c r="H44" s="56"/>
-      <c r="I44" s="56"/>
-      <c r="J44" s="56"/>
-      <c r="K44" s="56"/>
-      <c r="L44" s="56"/>
-      <c r="M44" s="56"/>
-      <c r="N44" s="56"/>
-      <c r="O44" s="56"/>
-      <c r="P44" s="56"/>
-      <c r="Q44" s="56"/>
-      <c r="R44" s="56"/>
-      <c r="S44" s="56"/>
-      <c r="T44" s="56"/>
-      <c r="U44" s="56"/>
-      <c r="V44" s="56"/>
-      <c r="W44" s="56"/>
-      <c r="X44" s="56"/>
-    </row>
-    <row r="45" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E44" s="87"/>
+      <c r="F44" s="87"/>
+      <c r="G44" s="87"/>
+      <c r="H44" s="87"/>
+      <c r="I44" s="87"/>
+      <c r="J44" s="87"/>
+      <c r="K44" s="87"/>
+      <c r="L44" s="87"/>
+      <c r="M44" s="87"/>
+      <c r="N44" s="87"/>
+      <c r="O44" s="87"/>
+      <c r="P44" s="87"/>
+      <c r="Q44" s="87"/>
+      <c r="R44" s="87"/>
+      <c r="S44" s="87"/>
+      <c r="T44" s="87"/>
+      <c r="U44" s="87"/>
+      <c r="V44" s="87"/>
+      <c r="W44" s="87"/>
+      <c r="X44" s="87"/>
+      <c r="Y44" s="84"/>
+      <c r="Z44" s="84"/>
+    </row>
+    <row r="45" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="56" t="s">
         <v>12</v>
       </c>
@@ -21867,28 +21981,30 @@
       <c r="D45" s="56" t="s">
         <v>106</v>
       </c>
-      <c r="E45" s="56"/>
-      <c r="F45" s="56"/>
-      <c r="G45" s="56"/>
-      <c r="H45" s="56"/>
-      <c r="I45" s="56"/>
-      <c r="J45" s="56"/>
-      <c r="K45" s="56"/>
-      <c r="L45" s="56"/>
-      <c r="M45" s="56"/>
-      <c r="N45" s="56"/>
-      <c r="O45" s="56"/>
-      <c r="P45" s="56"/>
-      <c r="Q45" s="56"/>
-      <c r="R45" s="56"/>
-      <c r="S45" s="56"/>
-      <c r="T45" s="56"/>
-      <c r="U45" s="56"/>
-      <c r="V45" s="56"/>
-      <c r="W45" s="56"/>
-      <c r="X45" s="56"/>
-    </row>
-    <row r="46" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E45" s="87"/>
+      <c r="F45" s="87"/>
+      <c r="G45" s="87"/>
+      <c r="H45" s="87"/>
+      <c r="I45" s="87"/>
+      <c r="J45" s="87"/>
+      <c r="K45" s="87"/>
+      <c r="L45" s="87"/>
+      <c r="M45" s="87"/>
+      <c r="N45" s="87"/>
+      <c r="O45" s="87"/>
+      <c r="P45" s="87"/>
+      <c r="Q45" s="87"/>
+      <c r="R45" s="87"/>
+      <c r="S45" s="87"/>
+      <c r="T45" s="87"/>
+      <c r="U45" s="87"/>
+      <c r="V45" s="87"/>
+      <c r="W45" s="87"/>
+      <c r="X45" s="87"/>
+      <c r="Y45" s="84"/>
+      <c r="Z45" s="84"/>
+    </row>
+    <row r="46" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="56" t="s">
         <v>15</v>
       </c>
@@ -21901,28 +22017,30 @@
       <c r="D46" s="56" t="s">
         <v>106</v>
       </c>
-      <c r="E46" s="56"/>
-      <c r="F46" s="56"/>
-      <c r="G46" s="56"/>
-      <c r="H46" s="56"/>
-      <c r="I46" s="56"/>
-      <c r="J46" s="56"/>
-      <c r="K46" s="56"/>
-      <c r="L46" s="56"/>
-      <c r="M46" s="56"/>
-      <c r="N46" s="56"/>
-      <c r="O46" s="56"/>
-      <c r="P46" s="56"/>
-      <c r="Q46" s="56"/>
-      <c r="R46" s="56"/>
-      <c r="S46" s="56"/>
-      <c r="T46" s="56"/>
-      <c r="U46" s="56"/>
-      <c r="V46" s="56"/>
-      <c r="W46" s="56"/>
-      <c r="X46" s="56"/>
-    </row>
-    <row r="47" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E46" s="87"/>
+      <c r="F46" s="87"/>
+      <c r="G46" s="87"/>
+      <c r="H46" s="87"/>
+      <c r="I46" s="87"/>
+      <c r="J46" s="87"/>
+      <c r="K46" s="87"/>
+      <c r="L46" s="87"/>
+      <c r="M46" s="87"/>
+      <c r="N46" s="87"/>
+      <c r="O46" s="87"/>
+      <c r="P46" s="87"/>
+      <c r="Q46" s="87"/>
+      <c r="R46" s="87"/>
+      <c r="S46" s="87"/>
+      <c r="T46" s="87"/>
+      <c r="U46" s="87"/>
+      <c r="V46" s="87"/>
+      <c r="W46" s="87"/>
+      <c r="X46" s="87"/>
+      <c r="Y46" s="84"/>
+      <c r="Z46" s="84"/>
+    </row>
+    <row r="47" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="56" t="s">
         <v>49</v>
       </c>
@@ -21933,28 +22051,30 @@
       <c r="D47" s="56" t="s">
         <v>105</v>
       </c>
-      <c r="E47" s="56"/>
-      <c r="F47" s="56"/>
-      <c r="G47" s="56"/>
-      <c r="H47" s="56"/>
-      <c r="I47" s="56"/>
-      <c r="J47" s="56"/>
-      <c r="K47" s="56"/>
-      <c r="L47" s="56"/>
-      <c r="M47" s="56"/>
-      <c r="N47" s="56"/>
-      <c r="O47" s="56"/>
-      <c r="P47" s="56"/>
-      <c r="Q47" s="56"/>
-      <c r="R47" s="56"/>
-      <c r="S47" s="56"/>
-      <c r="T47" s="56"/>
-      <c r="U47" s="56"/>
-      <c r="V47" s="56"/>
-      <c r="W47" s="56"/>
-      <c r="X47" s="56"/>
-    </row>
-    <row r="48" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E47" s="87"/>
+      <c r="F47" s="87"/>
+      <c r="G47" s="87"/>
+      <c r="H47" s="87"/>
+      <c r="I47" s="87"/>
+      <c r="J47" s="87"/>
+      <c r="K47" s="87"/>
+      <c r="L47" s="87"/>
+      <c r="M47" s="87"/>
+      <c r="N47" s="87"/>
+      <c r="O47" s="87"/>
+      <c r="P47" s="87"/>
+      <c r="Q47" s="87"/>
+      <c r="R47" s="87"/>
+      <c r="S47" s="87"/>
+      <c r="T47" s="87"/>
+      <c r="U47" s="87"/>
+      <c r="V47" s="87"/>
+      <c r="W47" s="87"/>
+      <c r="X47" s="87"/>
+      <c r="Y47" s="84"/>
+      <c r="Z47" s="84"/>
+    </row>
+    <row r="48" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="56" t="s">
         <v>9</v>
       </c>
@@ -21967,26 +22087,28 @@
       <c r="D48" s="56" t="s">
         <v>106</v>
       </c>
-      <c r="E48" s="56"/>
-      <c r="F48" s="56"/>
-      <c r="G48" s="56"/>
-      <c r="H48" s="56"/>
-      <c r="I48" s="56"/>
-      <c r="J48" s="56"/>
-      <c r="K48" s="56"/>
-      <c r="L48" s="56"/>
-      <c r="M48" s="56"/>
-      <c r="N48" s="56"/>
-      <c r="O48" s="56"/>
-      <c r="P48" s="56"/>
-      <c r="Q48" s="56"/>
-      <c r="R48" s="56"/>
-      <c r="S48" s="56"/>
-      <c r="T48" s="56"/>
-      <c r="U48" s="56"/>
-      <c r="V48" s="56"/>
-      <c r="W48" s="56"/>
-      <c r="X48" s="56"/>
+      <c r="E48" s="87"/>
+      <c r="F48" s="87"/>
+      <c r="G48" s="87"/>
+      <c r="H48" s="87"/>
+      <c r="I48" s="87"/>
+      <c r="J48" s="87"/>
+      <c r="K48" s="87"/>
+      <c r="L48" s="87"/>
+      <c r="M48" s="87"/>
+      <c r="N48" s="87"/>
+      <c r="O48" s="87"/>
+      <c r="P48" s="87"/>
+      <c r="Q48" s="87"/>
+      <c r="R48" s="87"/>
+      <c r="S48" s="87"/>
+      <c r="T48" s="87"/>
+      <c r="U48" s="87"/>
+      <c r="V48" s="87"/>
+      <c r="W48" s="87"/>
+      <c r="X48" s="87"/>
+      <c r="Y48" s="84"/>
+      <c r="Z48" s="84"/>
     </row>
     <row r="49" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="56" t="s">
@@ -22001,26 +22123,28 @@
       <c r="D49" s="56" t="s">
         <v>106</v>
       </c>
-      <c r="E49" s="56"/>
-      <c r="F49" s="56"/>
-      <c r="G49" s="56"/>
-      <c r="H49" s="56"/>
-      <c r="I49" s="56"/>
-      <c r="J49" s="56"/>
-      <c r="K49" s="56"/>
-      <c r="L49" s="56"/>
-      <c r="M49" s="56"/>
-      <c r="N49" s="56"/>
-      <c r="O49" s="56"/>
-      <c r="P49" s="56"/>
-      <c r="Q49" s="56"/>
-      <c r="R49" s="56"/>
-      <c r="S49" s="56"/>
-      <c r="T49" s="56"/>
-      <c r="U49" s="56"/>
-      <c r="V49" s="56"/>
-      <c r="W49" s="56"/>
-      <c r="X49" s="56"/>
+      <c r="E49" s="87"/>
+      <c r="F49" s="87"/>
+      <c r="G49" s="87"/>
+      <c r="H49" s="87"/>
+      <c r="I49" s="87"/>
+      <c r="J49" s="87"/>
+      <c r="K49" s="87"/>
+      <c r="L49" s="87"/>
+      <c r="M49" s="87"/>
+      <c r="N49" s="87"/>
+      <c r="O49" s="87"/>
+      <c r="P49" s="87"/>
+      <c r="Q49" s="87"/>
+      <c r="R49" s="87"/>
+      <c r="S49" s="87"/>
+      <c r="T49" s="87"/>
+      <c r="U49" s="87"/>
+      <c r="V49" s="87"/>
+      <c r="W49" s="87"/>
+      <c r="X49" s="87"/>
+      <c r="Y49" s="84"/>
+      <c r="Z49" s="84"/>
     </row>
     <row r="50" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="56" t="s">
@@ -22035,26 +22159,28 @@
       <c r="D50" s="56" t="s">
         <v>106</v>
       </c>
-      <c r="E50" s="56"/>
-      <c r="F50" s="56"/>
-      <c r="G50" s="56"/>
-      <c r="H50" s="56"/>
-      <c r="I50" s="56"/>
-      <c r="J50" s="56"/>
-      <c r="K50" s="56"/>
-      <c r="L50" s="56"/>
-      <c r="M50" s="56"/>
-      <c r="N50" s="56"/>
-      <c r="O50" s="56"/>
-      <c r="P50" s="56"/>
-      <c r="Q50" s="56"/>
-      <c r="R50" s="56"/>
-      <c r="S50" s="56"/>
-      <c r="T50" s="56"/>
-      <c r="U50" s="56"/>
-      <c r="V50" s="56"/>
-      <c r="W50" s="56"/>
-      <c r="X50" s="56"/>
+      <c r="E50" s="87"/>
+      <c r="F50" s="87"/>
+      <c r="G50" s="87"/>
+      <c r="H50" s="87"/>
+      <c r="I50" s="87"/>
+      <c r="J50" s="87"/>
+      <c r="K50" s="87"/>
+      <c r="L50" s="87"/>
+      <c r="M50" s="87"/>
+      <c r="N50" s="87"/>
+      <c r="O50" s="87"/>
+      <c r="P50" s="87"/>
+      <c r="Q50" s="87"/>
+      <c r="R50" s="87"/>
+      <c r="S50" s="87"/>
+      <c r="T50" s="87"/>
+      <c r="U50" s="87"/>
+      <c r="V50" s="87"/>
+      <c r="W50" s="87"/>
+      <c r="X50" s="87"/>
+      <c r="Y50" s="84"/>
+      <c r="Z50" s="84"/>
     </row>
     <row r="51" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A51" s="59" t="s">
@@ -22063,28 +22189,28 @@
       <c r="B51" s="60"/>
       <c r="C51" s="61"/>
       <c r="D51" s="60"/>
-      <c r="E51" s="60"/>
-      <c r="F51" s="60"/>
-      <c r="G51" s="60"/>
-      <c r="H51" s="60"/>
-      <c r="I51" s="60"/>
-      <c r="J51" s="60"/>
-      <c r="K51" s="60"/>
-      <c r="L51" s="60"/>
-      <c r="M51" s="60"/>
-      <c r="N51" s="60"/>
-      <c r="O51" s="60"/>
-      <c r="P51" s="60"/>
-      <c r="Q51" s="60"/>
-      <c r="R51" s="60"/>
-      <c r="S51" s="60"/>
-      <c r="T51" s="60"/>
-      <c r="U51" s="60"/>
-      <c r="V51" s="60"/>
-      <c r="W51" s="60"/>
-      <c r="X51" s="60"/>
-      <c r="Y51" s="60"/>
-      <c r="Z51" s="60"/>
+      <c r="E51" s="88"/>
+      <c r="F51" s="88"/>
+      <c r="G51" s="88"/>
+      <c r="H51" s="88"/>
+      <c r="I51" s="88"/>
+      <c r="J51" s="88"/>
+      <c r="K51" s="88"/>
+      <c r="L51" s="88"/>
+      <c r="M51" s="88"/>
+      <c r="N51" s="88"/>
+      <c r="O51" s="88"/>
+      <c r="P51" s="88"/>
+      <c r="Q51" s="88"/>
+      <c r="R51" s="88"/>
+      <c r="S51" s="88"/>
+      <c r="T51" s="88"/>
+      <c r="U51" s="88"/>
+      <c r="V51" s="88"/>
+      <c r="W51" s="88"/>
+      <c r="X51" s="88"/>
+      <c r="Y51" s="88"/>
+      <c r="Z51" s="88"/>
     </row>
     <row r="52" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="60" t="s">
@@ -22097,57 +22223,642 @@
       <c r="D52" s="63" t="s">
         <v>95</v>
       </c>
-      <c r="E52" s="60"/>
-      <c r="F52" s="60"/>
-      <c r="G52" s="60"/>
-      <c r="H52" s="60"/>
-      <c r="I52" s="60"/>
-      <c r="J52" s="60"/>
-      <c r="K52" s="60"/>
-      <c r="L52" s="60"/>
-      <c r="M52" s="60"/>
-      <c r="N52" s="60"/>
-      <c r="O52" s="60"/>
-      <c r="P52" s="60"/>
-      <c r="Q52" s="60"/>
-      <c r="R52" s="60"/>
-      <c r="S52" s="60"/>
-      <c r="T52" s="60"/>
-      <c r="U52" s="60"/>
-      <c r="V52" s="60"/>
-      <c r="W52" s="60"/>
-      <c r="X52" s="60"/>
-      <c r="Y52" s="60"/>
-      <c r="Z52" s="60"/>
-    </row>
-    <row r="53" spans="1:26" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="54" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="61" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="63" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="65" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="66" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="67" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="68" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="69" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="70" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="71" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="72" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="73" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="74" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="75" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="76" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="77" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="78" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="79" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="80" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="E52" s="88"/>
+      <c r="F52" s="88"/>
+      <c r="G52" s="88"/>
+      <c r="H52" s="88"/>
+      <c r="I52" s="88"/>
+      <c r="J52" s="88"/>
+      <c r="K52" s="88"/>
+      <c r="L52" s="88"/>
+      <c r="M52" s="88"/>
+      <c r="N52" s="88"/>
+      <c r="O52" s="88"/>
+      <c r="P52" s="88"/>
+      <c r="Q52" s="88"/>
+      <c r="R52" s="88"/>
+      <c r="S52" s="88"/>
+      <c r="T52" s="88"/>
+      <c r="U52" s="88"/>
+      <c r="V52" s="88"/>
+      <c r="W52" s="88"/>
+      <c r="X52" s="88"/>
+      <c r="Y52" s="88"/>
+      <c r="Z52" s="88"/>
+    </row>
+    <row r="53" spans="1:26" ht="21" x14ac:dyDescent="0.4">
+      <c r="A53" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="B53" s="40"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="40"/>
+      <c r="E53" s="84"/>
+      <c r="F53" s="84"/>
+      <c r="G53" s="84"/>
+      <c r="H53" s="84"/>
+      <c r="I53" s="84"/>
+      <c r="J53" s="84"/>
+      <c r="K53" s="84"/>
+      <c r="L53" s="84"/>
+      <c r="M53" s="84"/>
+      <c r="N53" s="84"/>
+      <c r="O53" s="84"/>
+      <c r="P53" s="84"/>
+      <c r="Q53" s="84"/>
+      <c r="R53" s="84"/>
+      <c r="S53" s="84"/>
+      <c r="T53" s="84"/>
+      <c r="U53" s="84"/>
+      <c r="V53" s="84"/>
+      <c r="W53" s="84"/>
+      <c r="X53" s="84"/>
+      <c r="Y53" s="84"/>
+      <c r="Z53" s="84"/>
+    </row>
+    <row r="54" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="43" t="s">
+        <v>345</v>
+      </c>
+      <c r="B54" s="90" t="s">
+        <v>357</v>
+      </c>
+      <c r="C54" s="43"/>
+      <c r="D54" s="81" t="s">
+        <v>347</v>
+      </c>
+      <c r="E54" s="84"/>
+      <c r="F54" s="84"/>
+      <c r="G54" s="84"/>
+      <c r="H54" s="84"/>
+      <c r="I54" s="84"/>
+      <c r="J54" s="84"/>
+      <c r="K54" s="84"/>
+      <c r="L54" s="84"/>
+      <c r="M54" s="84"/>
+      <c r="N54" s="84"/>
+      <c r="O54" s="84"/>
+      <c r="P54" s="84"/>
+      <c r="Q54" s="84"/>
+      <c r="R54" s="84"/>
+      <c r="S54" s="84"/>
+      <c r="T54" s="84"/>
+      <c r="U54" s="84"/>
+      <c r="V54" s="84"/>
+      <c r="W54" s="84"/>
+      <c r="X54" s="84"/>
+      <c r="Y54" s="84"/>
+      <c r="Z54" s="84"/>
+    </row>
+    <row r="55" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="43" t="s">
+        <v>346</v>
+      </c>
+      <c r="B55" s="81" t="s">
+        <v>358</v>
+      </c>
+      <c r="C55" s="43"/>
+      <c r="D55" s="81" t="s">
+        <v>348</v>
+      </c>
+      <c r="E55" s="84"/>
+      <c r="F55" s="84"/>
+      <c r="G55" s="84"/>
+      <c r="H55" s="84"/>
+      <c r="I55" s="84"/>
+      <c r="J55" s="84"/>
+      <c r="K55" s="84"/>
+      <c r="L55" s="84"/>
+      <c r="M55" s="84"/>
+      <c r="N55" s="84"/>
+      <c r="O55" s="84"/>
+      <c r="P55" s="84"/>
+      <c r="Q55" s="84"/>
+      <c r="R55" s="84"/>
+      <c r="S55" s="84"/>
+      <c r="T55" s="84"/>
+      <c r="U55" s="84"/>
+      <c r="V55" s="84"/>
+      <c r="W55" s="84"/>
+      <c r="X55" s="84"/>
+      <c r="Y55" s="84"/>
+      <c r="Z55" s="84"/>
+    </row>
+    <row r="56" spans="1:26" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A56" s="6" t="s">
+        <v>349</v>
+      </c>
+      <c r="B56" s="46"/>
+      <c r="C56" s="47"/>
+      <c r="D56" s="48" t="s">
+        <v>350</v>
+      </c>
+      <c r="E56" s="84"/>
+      <c r="F56" s="84"/>
+      <c r="G56" s="84"/>
+      <c r="H56" s="84"/>
+      <c r="I56" s="84"/>
+      <c r="J56" s="84"/>
+      <c r="K56" s="84"/>
+      <c r="L56" s="84"/>
+      <c r="M56" s="84"/>
+      <c r="N56" s="84"/>
+      <c r="O56" s="84"/>
+      <c r="P56" s="84"/>
+      <c r="Q56" s="84"/>
+      <c r="R56" s="84"/>
+      <c r="S56" s="84"/>
+      <c r="T56" s="84"/>
+      <c r="U56" s="84"/>
+      <c r="V56" s="84"/>
+      <c r="W56" s="84"/>
+      <c r="X56" s="84"/>
+      <c r="Y56" s="84"/>
+      <c r="Z56" s="84"/>
+    </row>
+    <row r="57" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="48" t="s">
+        <v>355</v>
+      </c>
+      <c r="B57" s="89" t="s">
+        <v>356</v>
+      </c>
+      <c r="C57" s="48"/>
+      <c r="D57" s="48"/>
+      <c r="E57" s="84"/>
+      <c r="F57" s="84"/>
+      <c r="G57" s="84"/>
+      <c r="H57" s="84"/>
+      <c r="I57" s="84"/>
+      <c r="J57" s="84"/>
+      <c r="K57" s="84"/>
+      <c r="L57" s="84"/>
+      <c r="M57" s="84"/>
+      <c r="N57" s="84"/>
+      <c r="O57" s="84"/>
+      <c r="P57" s="84"/>
+      <c r="Q57" s="84"/>
+      <c r="R57" s="84"/>
+      <c r="S57" s="84"/>
+      <c r="T57" s="84"/>
+      <c r="U57" s="84"/>
+      <c r="V57" s="84"/>
+      <c r="W57" s="84"/>
+      <c r="X57" s="84"/>
+      <c r="Y57" s="84"/>
+      <c r="Z57" s="84"/>
+    </row>
+    <row r="58" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="48" t="s">
+        <v>351</v>
+      </c>
+      <c r="B58" s="82">
+        <v>3175</v>
+      </c>
+      <c r="C58" s="47"/>
+      <c r="D58" s="49" t="s">
+        <v>354</v>
+      </c>
+      <c r="E58" s="84"/>
+      <c r="F58" s="84"/>
+      <c r="G58" s="84"/>
+      <c r="H58" s="84"/>
+      <c r="I58" s="84"/>
+      <c r="J58" s="84"/>
+      <c r="K58" s="84"/>
+      <c r="L58" s="84"/>
+      <c r="M58" s="84"/>
+      <c r="N58" s="84"/>
+      <c r="O58" s="84"/>
+      <c r="P58" s="84"/>
+      <c r="Q58" s="84"/>
+      <c r="R58" s="84"/>
+      <c r="S58" s="84"/>
+      <c r="T58" s="84"/>
+      <c r="U58" s="84"/>
+      <c r="V58" s="84"/>
+      <c r="W58" s="84"/>
+      <c r="X58" s="84"/>
+      <c r="Y58" s="84"/>
+      <c r="Z58" s="84"/>
+    </row>
+    <row r="59" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="48" t="s">
+        <v>352</v>
+      </c>
+      <c r="B59" s="82">
+        <v>1208</v>
+      </c>
+      <c r="C59" s="47"/>
+      <c r="D59" s="49" t="s">
+        <v>353</v>
+      </c>
+      <c r="E59" s="84"/>
+      <c r="F59" s="84"/>
+      <c r="G59" s="84"/>
+      <c r="H59" s="84"/>
+      <c r="I59" s="84"/>
+      <c r="J59" s="84"/>
+      <c r="K59" s="84"/>
+      <c r="L59" s="84"/>
+      <c r="M59" s="84"/>
+      <c r="N59" s="84"/>
+      <c r="O59" s="84"/>
+      <c r="P59" s="84"/>
+      <c r="Q59" s="84"/>
+      <c r="R59" s="84"/>
+      <c r="S59" s="84"/>
+      <c r="T59" s="84"/>
+      <c r="U59" s="84"/>
+      <c r="V59" s="84"/>
+      <c r="W59" s="84"/>
+      <c r="X59" s="84"/>
+      <c r="Y59" s="84"/>
+      <c r="Z59" s="84"/>
+    </row>
+    <row r="60" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="48" t="s">
+        <v>351</v>
+      </c>
+      <c r="B60" s="82">
+        <v>2411</v>
+      </c>
+      <c r="C60" s="47"/>
+      <c r="D60" s="49" t="s">
+        <v>354</v>
+      </c>
+      <c r="E60" s="84"/>
+      <c r="F60" s="84"/>
+      <c r="G60" s="84"/>
+      <c r="H60" s="84"/>
+      <c r="I60" s="84"/>
+      <c r="J60" s="84"/>
+      <c r="K60" s="84"/>
+      <c r="L60" s="84"/>
+      <c r="M60" s="84"/>
+      <c r="N60" s="84"/>
+      <c r="O60" s="84"/>
+      <c r="P60" s="84"/>
+      <c r="Q60" s="84"/>
+      <c r="R60" s="84"/>
+      <c r="S60" s="84"/>
+      <c r="T60" s="84"/>
+      <c r="U60" s="84"/>
+      <c r="V60" s="84"/>
+      <c r="W60" s="84"/>
+      <c r="X60" s="84"/>
+      <c r="Y60" s="84"/>
+      <c r="Z60" s="84"/>
+    </row>
+    <row r="61" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="48" t="s">
+        <v>352</v>
+      </c>
+      <c r="B61" s="82">
+        <v>1427</v>
+      </c>
+      <c r="C61" s="47"/>
+      <c r="D61" s="49" t="s">
+        <v>353</v>
+      </c>
+      <c r="E61" s="84"/>
+      <c r="F61" s="84"/>
+      <c r="G61" s="84"/>
+      <c r="H61" s="84"/>
+      <c r="I61" s="84"/>
+      <c r="J61" s="84"/>
+      <c r="K61" s="84"/>
+      <c r="L61" s="84"/>
+      <c r="M61" s="84"/>
+      <c r="N61" s="84"/>
+      <c r="O61" s="84"/>
+      <c r="P61" s="84"/>
+      <c r="Q61" s="84"/>
+      <c r="R61" s="84"/>
+      <c r="S61" s="84"/>
+      <c r="T61" s="84"/>
+      <c r="U61" s="84"/>
+      <c r="V61" s="84"/>
+      <c r="W61" s="84"/>
+      <c r="X61" s="84"/>
+      <c r="Y61" s="84"/>
+      <c r="Z61" s="84"/>
+    </row>
+    <row r="62" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="48" t="s">
+        <v>351</v>
+      </c>
+      <c r="B62" s="82">
+        <v>2934</v>
+      </c>
+      <c r="C62" s="47"/>
+      <c r="D62" s="49" t="s">
+        <v>354</v>
+      </c>
+      <c r="E62" s="84"/>
+      <c r="F62" s="84"/>
+      <c r="G62" s="84"/>
+      <c r="H62" s="84"/>
+      <c r="I62" s="84"/>
+      <c r="J62" s="84"/>
+      <c r="K62" s="84"/>
+      <c r="L62" s="84"/>
+      <c r="M62" s="84"/>
+      <c r="N62" s="84"/>
+      <c r="O62" s="84"/>
+      <c r="P62" s="84"/>
+      <c r="Q62" s="84"/>
+      <c r="R62" s="84"/>
+      <c r="S62" s="84"/>
+      <c r="T62" s="84"/>
+      <c r="U62" s="84"/>
+      <c r="V62" s="84"/>
+      <c r="W62" s="84"/>
+      <c r="X62" s="84"/>
+      <c r="Y62" s="84"/>
+      <c r="Z62" s="84"/>
+    </row>
+    <row r="63" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="48" t="s">
+        <v>352</v>
+      </c>
+      <c r="B63" s="82">
+        <v>1245</v>
+      </c>
+      <c r="C63" s="47"/>
+      <c r="D63" s="49" t="s">
+        <v>353</v>
+      </c>
+      <c r="E63" s="84"/>
+      <c r="F63" s="84"/>
+      <c r="G63" s="84"/>
+      <c r="H63" s="84"/>
+      <c r="I63" s="84"/>
+      <c r="J63" s="84"/>
+      <c r="K63" s="84"/>
+      <c r="L63" s="84"/>
+      <c r="M63" s="84"/>
+      <c r="N63" s="84"/>
+      <c r="O63" s="84"/>
+      <c r="P63" s="84"/>
+      <c r="Q63" s="84"/>
+      <c r="R63" s="84"/>
+      <c r="S63" s="84"/>
+      <c r="T63" s="84"/>
+      <c r="U63" s="84"/>
+      <c r="V63" s="84"/>
+      <c r="W63" s="84"/>
+      <c r="X63" s="84"/>
+      <c r="Y63" s="84"/>
+      <c r="Z63" s="84"/>
+    </row>
+    <row r="64" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E64" s="84"/>
+      <c r="F64" s="84"/>
+      <c r="G64" s="84"/>
+      <c r="H64" s="84"/>
+      <c r="I64" s="84"/>
+      <c r="J64" s="84"/>
+      <c r="K64" s="84"/>
+      <c r="L64" s="84"/>
+      <c r="M64" s="84"/>
+      <c r="N64" s="84"/>
+      <c r="O64" s="84"/>
+      <c r="P64" s="84"/>
+      <c r="Q64" s="84"/>
+      <c r="R64" s="84"/>
+      <c r="S64" s="84"/>
+      <c r="T64" s="84"/>
+      <c r="U64" s="84"/>
+      <c r="V64" s="84"/>
+      <c r="W64" s="84"/>
+      <c r="X64" s="84"/>
+      <c r="Y64" s="84"/>
+      <c r="Z64" s="84"/>
+    </row>
+    <row r="65" spans="5:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E65" s="84"/>
+      <c r="F65" s="84"/>
+      <c r="G65" s="84"/>
+      <c r="H65" s="84"/>
+      <c r="I65" s="84"/>
+      <c r="J65" s="84"/>
+      <c r="K65" s="84"/>
+      <c r="L65" s="84"/>
+      <c r="M65" s="84"/>
+      <c r="N65" s="84"/>
+      <c r="O65" s="84"/>
+      <c r="P65" s="84"/>
+      <c r="Q65" s="84"/>
+      <c r="R65" s="84"/>
+      <c r="S65" s="84"/>
+      <c r="T65" s="84"/>
+      <c r="U65" s="84"/>
+      <c r="V65" s="84"/>
+      <c r="W65" s="84"/>
+      <c r="X65" s="84"/>
+      <c r="Y65" s="84"/>
+      <c r="Z65" s="84"/>
+    </row>
+    <row r="66" spans="5:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E66" s="84"/>
+      <c r="F66" s="84"/>
+      <c r="G66" s="84"/>
+      <c r="H66" s="84"/>
+      <c r="I66" s="84"/>
+      <c r="J66" s="84"/>
+      <c r="K66" s="84"/>
+      <c r="L66" s="84"/>
+      <c r="M66" s="84"/>
+      <c r="N66" s="84"/>
+      <c r="O66" s="84"/>
+      <c r="P66" s="84"/>
+      <c r="Q66" s="84"/>
+      <c r="R66" s="84"/>
+      <c r="S66" s="84"/>
+      <c r="T66" s="84"/>
+      <c r="U66" s="84"/>
+      <c r="V66" s="84"/>
+      <c r="W66" s="84"/>
+      <c r="X66" s="84"/>
+      <c r="Y66" s="84"/>
+      <c r="Z66" s="84"/>
+    </row>
+    <row r="67" spans="5:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E67" s="84"/>
+      <c r="F67" s="84"/>
+      <c r="G67" s="84"/>
+      <c r="H67" s="84"/>
+      <c r="I67" s="84"/>
+      <c r="J67" s="84"/>
+      <c r="K67" s="84"/>
+      <c r="L67" s="84"/>
+      <c r="M67" s="84"/>
+      <c r="N67" s="84"/>
+      <c r="O67" s="84"/>
+      <c r="P67" s="84"/>
+      <c r="Q67" s="84"/>
+      <c r="R67" s="84"/>
+      <c r="S67" s="84"/>
+      <c r="T67" s="84"/>
+      <c r="U67" s="84"/>
+      <c r="V67" s="84"/>
+      <c r="W67" s="84"/>
+      <c r="X67" s="84"/>
+      <c r="Y67" s="84"/>
+      <c r="Z67" s="84"/>
+    </row>
+    <row r="68" spans="5:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E68" s="84"/>
+      <c r="F68" s="84"/>
+      <c r="G68" s="84"/>
+      <c r="H68" s="84"/>
+      <c r="I68" s="84"/>
+      <c r="J68" s="84"/>
+      <c r="K68" s="84"/>
+      <c r="L68" s="84"/>
+      <c r="M68" s="84"/>
+      <c r="N68" s="84"/>
+      <c r="O68" s="84"/>
+      <c r="P68" s="84"/>
+      <c r="Q68" s="84"/>
+      <c r="R68" s="84"/>
+      <c r="S68" s="84"/>
+      <c r="T68" s="84"/>
+      <c r="U68" s="84"/>
+      <c r="V68" s="84"/>
+      <c r="W68" s="84"/>
+      <c r="X68" s="84"/>
+      <c r="Y68" s="84"/>
+      <c r="Z68" s="84"/>
+    </row>
+    <row r="69" spans="5:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E69" s="84"/>
+      <c r="F69" s="84"/>
+      <c r="G69" s="84"/>
+      <c r="H69" s="84"/>
+      <c r="I69" s="84"/>
+      <c r="J69" s="84"/>
+      <c r="K69" s="84"/>
+      <c r="L69" s="84"/>
+      <c r="M69" s="84"/>
+      <c r="N69" s="84"/>
+      <c r="O69" s="84"/>
+      <c r="P69" s="84"/>
+      <c r="Q69" s="84"/>
+      <c r="R69" s="84"/>
+      <c r="S69" s="84"/>
+      <c r="T69" s="84"/>
+      <c r="U69" s="84"/>
+      <c r="V69" s="84"/>
+      <c r="W69" s="84"/>
+      <c r="X69" s="84"/>
+      <c r="Y69" s="84"/>
+      <c r="Z69" s="84"/>
+    </row>
+    <row r="70" spans="5:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E70" s="84"/>
+      <c r="F70" s="84"/>
+      <c r="G70" s="84"/>
+      <c r="H70" s="84"/>
+      <c r="I70" s="84"/>
+      <c r="J70" s="84"/>
+      <c r="K70" s="84"/>
+      <c r="L70" s="84"/>
+      <c r="M70" s="84"/>
+      <c r="N70" s="84"/>
+      <c r="O70" s="84"/>
+      <c r="P70" s="84"/>
+      <c r="Q70" s="84"/>
+      <c r="R70" s="84"/>
+      <c r="S70" s="84"/>
+      <c r="T70" s="84"/>
+      <c r="U70" s="84"/>
+      <c r="V70" s="84"/>
+      <c r="W70" s="84"/>
+      <c r="X70" s="84"/>
+      <c r="Y70" s="84"/>
+      <c r="Z70" s="84"/>
+    </row>
+    <row r="71" spans="5:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E71" s="84"/>
+      <c r="F71" s="84"/>
+      <c r="G71" s="84"/>
+      <c r="H71" s="84"/>
+      <c r="I71" s="84"/>
+      <c r="J71" s="84"/>
+      <c r="K71" s="84"/>
+      <c r="L71" s="84"/>
+      <c r="M71" s="84"/>
+      <c r="N71" s="84"/>
+      <c r="O71" s="84"/>
+      <c r="P71" s="84"/>
+      <c r="Q71" s="84"/>
+      <c r="R71" s="84"/>
+      <c r="S71" s="84"/>
+      <c r="T71" s="84"/>
+      <c r="U71" s="84"/>
+      <c r="V71" s="84"/>
+      <c r="W71" s="84"/>
+      <c r="X71" s="84"/>
+      <c r="Y71" s="84"/>
+      <c r="Z71" s="84"/>
+    </row>
+    <row r="72" spans="5:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E72" s="84"/>
+      <c r="F72" s="84"/>
+      <c r="G72" s="84"/>
+      <c r="H72" s="84"/>
+      <c r="I72" s="84"/>
+      <c r="J72" s="84"/>
+      <c r="K72" s="84"/>
+      <c r="L72" s="84"/>
+      <c r="M72" s="84"/>
+      <c r="N72" s="84"/>
+      <c r="O72" s="84"/>
+      <c r="P72" s="84"/>
+      <c r="Q72" s="84"/>
+      <c r="R72" s="84"/>
+      <c r="S72" s="84"/>
+      <c r="T72" s="84"/>
+      <c r="U72" s="84"/>
+      <c r="V72" s="84"/>
+      <c r="W72" s="84"/>
+      <c r="X72" s="84"/>
+      <c r="Y72" s="84"/>
+      <c r="Z72" s="84"/>
+    </row>
+    <row r="73" spans="5:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E73" s="84"/>
+      <c r="F73" s="84"/>
+      <c r="G73" s="84"/>
+      <c r="H73" s="84"/>
+      <c r="I73" s="84"/>
+      <c r="J73" s="84"/>
+      <c r="K73" s="84"/>
+      <c r="L73" s="84"/>
+      <c r="M73" s="84"/>
+      <c r="N73" s="84"/>
+      <c r="O73" s="84"/>
+      <c r="P73" s="84"/>
+      <c r="Q73" s="84"/>
+      <c r="R73" s="84"/>
+      <c r="S73" s="84"/>
+      <c r="T73" s="84"/>
+      <c r="U73" s="84"/>
+      <c r="V73" s="84"/>
+      <c r="W73" s="84"/>
+      <c r="X73" s="84"/>
+      <c r="Y73" s="84"/>
+      <c r="Z73" s="84"/>
+    </row>
+    <row r="74" spans="5:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" spans="5:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" spans="5:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" spans="5:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" spans="5:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" spans="5:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" spans="5:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="81" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="82" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="83" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -23071,7 +23782,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DD610E5-7CFE-40D9-832A-CDCE1C3A467E}">
   <dimension ref="A1:N50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
new registration function; target_mask for each target_image
</commit_message>
<xml_diff>
--- a/Database/CoastSnapDB.xlsx
+++ b/Database/CoastSnapDB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\CoastSnap\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EFA28E7-E4D2-4A2F-9EDA-FD3839222DAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE36E9F6-21D1-4602-9FE4-01E54A17DF0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3384" yWindow="1956" windowWidth="17280" windowHeight="8976" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="database" sheetId="1" r:id="rId1"/>
@@ -20450,8 +20450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C82C2A5-FA5F-4BBC-B066-D9DA22911E90}">
   <dimension ref="A1:Z993"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>